<commit_message>
Add reviewed tweets REVIEWED_RandyFeenstra_20201027_20210126_20250924.xlsx
</commit_message>
<xml_diff>
--- a/REVIEWED_RandyFeenstra_20201027_20210126_20250924.xlsx
+++ b/REVIEWED_RandyFeenstra_20201027_20210126_20250924.xlsx
@@ -608,10 +608,10 @@
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -643,10 +643,10 @@
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -680,10 +680,10 @@
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -812,10 +812,10 @@
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -973,10 +973,10 @@
       <c r="F16" t="inlineStr"/>
       <c r="G16" t="inlineStr"/>
       <c r="H16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
@@ -1010,10 +1010,10 @@
       <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr"/>
       <c r="H17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
@@ -1045,10 +1045,10 @@
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr"/>
       <c r="H18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19">
@@ -1144,10 +1144,10 @@
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22">
@@ -1175,10 +1175,10 @@
       <c r="F22" t="inlineStr"/>
       <c r="G22" t="inlineStr"/>
       <c r="H22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23">
@@ -1268,10 +1268,10 @@
       <c r="F25" t="inlineStr"/>
       <c r="G25" t="inlineStr"/>
       <c r="H25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26">

</xml_diff>